<commit_message>
Position de la bille
</commit_message>
<xml_diff>
--- a/doc/traitement_image_justif.xlsx
+++ b/doc/traitement_image_justif.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e42ac6eff042a85/documents/universite/s4/projet/projet_s4/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\projet_s4\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Sphere Template</t>
   </si>
@@ -108,13 +108,31 @@
   </si>
   <si>
     <t>v0: Image sans la sphere</t>
+  </si>
+  <si>
+    <t>s7</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>s9</t>
+  </si>
+  <si>
+    <t>s10</t>
+  </si>
+  <si>
+    <t>s11</t>
+  </si>
+  <si>
+    <t>s12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,8 +148,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,30 +170,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -235,41 +241,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,32 +311,66 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,723 +685,1516 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:AA21"/>
+  <dimension ref="A5:AG26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="D5" s="11" t="s">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="3"/>
     </row>
-    <row r="6" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="D6" s="11" t="s">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="10" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="10" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="10" t="s">
+      <c r="O6" s="9"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="9"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="11"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="10" t="s">
+      <c r="W6" s="9"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="W6" s="11"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="13" t="s">
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="33"/>
     </row>
-    <row r="7" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="D7" s="31" t="s">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="D7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="E7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="G7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="H7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="I7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="30" t="s">
+      <c r="M7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="27" t="s">
+      <c r="P7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="30" t="s">
+      <c r="Q7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="31" t="s">
+      <c r="S7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="27" t="s">
+      <c r="T7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="U7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="V7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="T7" s="31" t="s">
+      <c r="W7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="U7" s="27" t="s">
+      <c r="X7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="V7" s="30" t="s">
+      <c r="Y7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="AA7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="X7" s="27" t="s">
+      <c r="AB7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="29" t="s">
+      <c r="AC7" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AE7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AA7" s="28" t="s">
+      <c r="AF7" s="26" t="s">
         <v>18</v>
       </c>
+      <c r="AG7" s="27" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="8" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="30"/>
     </row>
-    <row r="9" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="19">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15">
         <v>0.59955999999999998</v>
       </c>
-      <c r="E9" s="2">
+      <c r="C9" s="15">
         <v>0.66700999999999999</v>
       </c>
-      <c r="F9" s="34">
+      <c r="D9" s="16">
         <v>0.73199999999999998</v>
       </c>
-      <c r="G9" s="22">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="25">
-        <v>1</v>
-      </c>
-      <c r="J9" s="22">
+      <c r="E9" s="29">
+        <f>AVERAGE(B9:D9)</f>
+        <v>0.66618999999999995</v>
+      </c>
+      <c r="F9" s="17">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15">
+        <v>1</v>
+      </c>
+      <c r="H9" s="16">
+        <v>1</v>
+      </c>
+      <c r="I9" s="29">
+        <f>AVERAGE(F9:H9)</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="17">
         <v>0.68530999999999997</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="15">
         <v>0.72280999999999995</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="16">
         <v>0.80683000000000005</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="29">
+        <f>AVERAGE(J9:L9)</f>
+        <v>0.73831666666666662</v>
+      </c>
+      <c r="N9" s="17">
         <v>0.71728000000000003</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="15">
         <v>0.75800999999999996</v>
       </c>
-      <c r="O9" s="25">
+      <c r="P9" s="16">
         <v>0.86772000000000005</v>
       </c>
-      <c r="P9" s="22">
+      <c r="Q9" s="29">
+        <f>AVERAGE(N9:P9)</f>
+        <v>0.78100333333333338</v>
+      </c>
+      <c r="R9" s="17">
         <v>0.53776999999999997</v>
       </c>
-      <c r="Q9" s="20">
+      <c r="S9" s="15">
         <v>0.58628999999999998</v>
       </c>
-      <c r="R9" s="6">
+      <c r="T9" s="16">
         <v>0.55859999999999999</v>
       </c>
-      <c r="S9" s="8">
+      <c r="U9" s="29">
+        <f>AVERAGE(R9:T9)</f>
+        <v>0.56088666666666664</v>
+      </c>
+      <c r="V9" s="17">
         <v>0.55708999999999997</v>
       </c>
-      <c r="T9" s="20">
+      <c r="W9" s="15">
         <v>0.57808000000000004</v>
       </c>
-      <c r="U9" s="23">
+      <c r="X9" s="16">
         <v>0.53876000000000002</v>
       </c>
-      <c r="V9" s="22">
+      <c r="Y9" s="29">
+        <f>AVERAGE(V9:X9)</f>
+        <v>0.55797666666666668</v>
+      </c>
+      <c r="Z9" s="17">
         <v>0.53776999999999997</v>
       </c>
-      <c r="W9" s="20">
+      <c r="AA9" s="15">
         <v>0.58628999999999998</v>
       </c>
-      <c r="X9" s="6">
+      <c r="AB9" s="16">
         <v>0.55859999999999999</v>
       </c>
-      <c r="Y9" s="24">
+      <c r="AC9" s="29">
+        <f>AVERAGE(Z9:AB9)</f>
+        <v>0.56088666666666664</v>
+      </c>
+      <c r="AD9" s="18">
         <v>0.54745999999999995</v>
       </c>
-      <c r="Z9" s="20">
+      <c r="AE9" s="15">
         <v>0.58104999999999996</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AF9" s="16">
         <v>0.57286000000000004</v>
       </c>
+      <c r="AG9" s="31">
+        <f>AVERAGE(AD9:AF9)</f>
+        <v>0.56712333333333331</v>
+      </c>
     </row>
-    <row r="10" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="32">
+      <c r="B10" s="15">
         <v>0.46348</v>
       </c>
-      <c r="E10" s="2">
+      <c r="C10" s="15">
         <v>0.49134</v>
       </c>
-      <c r="F10" s="25">
+      <c r="D10" s="16">
         <v>0.64434000000000002</v>
       </c>
-      <c r="G10" s="8">
+      <c r="E10" s="29">
+        <f t="shared" ref="E10:E15" si="0">AVERAGE(B10:D10)</f>
+        <v>0.53305333333333327</v>
+      </c>
+      <c r="F10" s="17">
         <v>0.70379000000000003</v>
       </c>
-      <c r="H10" s="19">
+      <c r="G10" s="15">
         <v>0.67593000000000003</v>
       </c>
-      <c r="I10" s="25">
+      <c r="H10" s="16">
         <v>0.79295000000000004</v>
       </c>
-      <c r="J10" s="22">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="25">
-        <v>1</v>
-      </c>
-      <c r="M10" s="22">
+      <c r="I10" s="29">
+        <f t="shared" ref="I10:I15" si="1">AVERAGE(F10:H10)</f>
+        <v>0.72422333333333333</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1</v>
+      </c>
+      <c r="K10" s="15">
+        <v>1</v>
+      </c>
+      <c r="L10" s="16">
+        <v>1</v>
+      </c>
+      <c r="M10" s="29">
+        <f t="shared" ref="M10:M15" si="2">AVERAGE(J10:L10)</f>
+        <v>1</v>
+      </c>
+      <c r="N10" s="17">
         <v>0.80552000000000001</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="15">
         <v>0.84616000000000002</v>
       </c>
-      <c r="O10" s="25">
+      <c r="P10" s="16">
         <v>0.85672999999999999</v>
       </c>
-      <c r="P10" s="33">
+      <c r="Q10" s="29">
+        <f t="shared" ref="Q10:Q15" si="3">AVERAGE(N10:P10)</f>
+        <v>0.83613666666666664</v>
+      </c>
+      <c r="R10" s="17">
         <v>0.46181</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="S10" s="15">
         <v>0.50295999999999996</v>
       </c>
-      <c r="R10" s="25">
+      <c r="T10" s="16">
         <v>0.53508</v>
       </c>
-      <c r="S10" s="22">
+      <c r="U10" s="29">
+        <f t="shared" ref="U10:U15" si="4">AVERAGE(R10:T10)</f>
+        <v>0.49994999999999995</v>
+      </c>
+      <c r="V10" s="17">
         <v>0.46459</v>
       </c>
-      <c r="T10" s="2">
+      <c r="W10" s="15">
         <v>0.49968000000000001</v>
       </c>
-      <c r="U10" s="25">
+      <c r="X10" s="16">
         <v>0.55547999999999997</v>
       </c>
-      <c r="V10" s="22">
+      <c r="Y10" s="29">
+        <f t="shared" ref="Y10:Y15" si="5">AVERAGE(V10:X10)</f>
+        <v>0.50658333333333327</v>
+      </c>
+      <c r="Z10" s="17">
         <v>0.47959000000000002</v>
       </c>
-      <c r="W10" s="2">
+      <c r="AA10" s="15">
         <v>0.65664999999999996</v>
       </c>
-      <c r="X10" s="25">
+      <c r="AB10" s="16">
         <v>0.72945000000000004</v>
       </c>
-      <c r="Y10" s="24">
+      <c r="AC10" s="29">
+        <f t="shared" ref="AC10:AC15" si="6">AVERAGE(Z10:AB10)</f>
+        <v>0.62189666666666665</v>
+      </c>
+      <c r="AD10" s="18">
         <v>0.45873000000000003</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="AE10" s="15">
         <v>0.55359999999999998</v>
       </c>
-      <c r="AA10" s="20">
+      <c r="AF10" s="16">
         <v>0.58608000000000005</v>
       </c>
+      <c r="AG10" s="31">
+        <f t="shared" ref="AG10:AG15" si="7">AVERAGE(AD10:AF10)</f>
+        <v>0.5328033333333333</v>
+      </c>
     </row>
-    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="19">
+      <c r="B11" s="15">
         <v>0.48125000000000001</v>
       </c>
-      <c r="E11" s="2">
+      <c r="C11" s="15">
         <v>0.48437999999999998</v>
       </c>
-      <c r="F11" s="25">
+      <c r="D11" s="16">
         <v>0.62144999999999995</v>
       </c>
-      <c r="G11" s="2">
+      <c r="E11" s="29">
+        <f t="shared" si="0"/>
+        <v>0.52902666666666665</v>
+      </c>
+      <c r="F11" s="15">
         <v>0.73936000000000002</v>
       </c>
-      <c r="H11" s="19">
+      <c r="G11" s="15">
         <v>0.68193000000000004</v>
       </c>
-      <c r="I11" s="34">
+      <c r="H11" s="16">
         <v>0.84104999999999996</v>
       </c>
-      <c r="J11" s="19">
+      <c r="I11" s="29">
+        <f t="shared" si="1"/>
+        <v>0.7541133333333333</v>
+      </c>
+      <c r="J11" s="15">
         <v>0.81457999999999997</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="15">
         <v>0.84662000000000004</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="16">
         <v>0.85858000000000001</v>
       </c>
-      <c r="M11" s="19">
-        <v>1</v>
-      </c>
-      <c r="N11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="34">
-        <v>1</v>
-      </c>
-      <c r="P11" s="5">
+      <c r="M11" s="29">
+        <f t="shared" si="2"/>
+        <v>0.8399266666666666</v>
+      </c>
+      <c r="N11" s="15">
+        <v>1</v>
+      </c>
+      <c r="O11" s="15">
+        <v>1</v>
+      </c>
+      <c r="P11" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="29">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R11" s="18">
         <v>0.51287000000000005</v>
       </c>
-      <c r="Q11" s="19">
+      <c r="S11" s="15">
         <v>0.51082000000000005</v>
       </c>
-      <c r="R11" s="34">
+      <c r="T11" s="16">
         <v>0.57643</v>
       </c>
-      <c r="S11" s="8">
+      <c r="U11" s="29">
+        <f t="shared" si="4"/>
+        <v>0.53337333333333337</v>
+      </c>
+      <c r="V11" s="17">
         <v>0.57759000000000005</v>
       </c>
-      <c r="T11" s="19">
+      <c r="W11" s="15">
         <v>0.51998999999999995</v>
       </c>
-      <c r="U11" s="25">
+      <c r="X11" s="16">
         <v>0.58655000000000002</v>
       </c>
-      <c r="V11" s="22">
+      <c r="Y11" s="29">
+        <f t="shared" si="5"/>
+        <v>0.56137666666666675</v>
+      </c>
+      <c r="Z11" s="17">
         <v>0.51251999999999998</v>
       </c>
-      <c r="W11" s="2">
+      <c r="AA11" s="15">
         <v>0.52927000000000002</v>
       </c>
-      <c r="X11" s="25">
+      <c r="AB11" s="16">
         <v>0.57643</v>
       </c>
-      <c r="Y11" s="24">
+      <c r="AC11" s="29">
+        <f t="shared" si="6"/>
+        <v>0.5394066666666667</v>
+      </c>
+      <c r="AD11" s="18">
         <v>0.52073999999999998</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="AE11" s="15">
         <v>0.52122000000000002</v>
       </c>
-      <c r="AA11" s="20">
+      <c r="AF11" s="16">
         <v>0.60070999999999997</v>
       </c>
+      <c r="AG11" s="31">
+        <f t="shared" si="7"/>
+        <v>0.54755666666666658</v>
+      </c>
     </row>
-    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="19">
+      <c r="B12" s="15">
         <v>0.56201999999999996</v>
       </c>
-      <c r="E12" s="2">
+      <c r="C12" s="15">
         <v>0.71235999999999999</v>
       </c>
-      <c r="F12" s="25">
+      <c r="D12" s="16">
         <v>0.71316000000000002</v>
       </c>
-      <c r="G12" s="22">
+      <c r="E12" s="29">
+        <f t="shared" si="0"/>
+        <v>0.66251333333333329</v>
+      </c>
+      <c r="F12" s="17">
         <v>0.56432000000000004</v>
       </c>
-      <c r="H12" s="2">
+      <c r="G12" s="15">
         <v>0.71016999999999997</v>
       </c>
-      <c r="I12" s="25">
+      <c r="H12" s="16">
         <v>0.71858999999999995</v>
       </c>
-      <c r="J12" s="22">
+      <c r="I12" s="29">
+        <f t="shared" si="1"/>
+        <v>0.66435999999999995</v>
+      </c>
+      <c r="J12" s="17">
         <v>0.56215999999999999</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="15">
         <v>0.71235999999999999</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="16">
         <v>0.71316000000000002</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="29">
+        <f t="shared" si="2"/>
+        <v>0.66255999999999993</v>
+      </c>
+      <c r="N12" s="17">
         <v>0.56540000000000001</v>
       </c>
-      <c r="N12" s="20">
+      <c r="O12" s="15">
         <v>0.72750000000000004</v>
       </c>
-      <c r="O12" s="6">
+      <c r="P12" s="16">
         <v>0.69340999999999997</v>
       </c>
-      <c r="P12" s="22">
+      <c r="Q12" s="29">
+        <f t="shared" si="3"/>
+        <v>0.66210333333333338</v>
+      </c>
+      <c r="R12" s="17">
         <v>0.57667999999999997</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="S12" s="15">
         <v>0.72575000000000001</v>
       </c>
-      <c r="R12" s="6">
+      <c r="T12" s="16">
         <v>0.66903999999999997</v>
       </c>
-      <c r="S12" s="22">
-        <v>1</v>
-      </c>
-      <c r="T12" s="2">
-        <v>1</v>
-      </c>
-      <c r="U12" s="25">
-        <v>1</v>
-      </c>
-      <c r="V12" s="8">
+      <c r="U12" s="29">
+        <f t="shared" si="4"/>
+        <v>0.65715666666666672</v>
+      </c>
+      <c r="V12" s="17">
+        <v>1</v>
+      </c>
+      <c r="W12" s="15">
+        <v>1</v>
+      </c>
+      <c r="X12" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="29">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Z12" s="17">
         <v>0.57681000000000004</v>
       </c>
-      <c r="W12" s="20">
+      <c r="AA12" s="15">
         <v>0.72575000000000001</v>
       </c>
-      <c r="X12" s="23">
+      <c r="AB12" s="16">
         <v>0.66903999999999997</v>
       </c>
-      <c r="Y12" s="24">
+      <c r="AC12" s="29">
+        <f t="shared" si="6"/>
+        <v>0.65720000000000001</v>
+      </c>
+      <c r="AD12" s="18">
         <v>0.57855000000000001</v>
       </c>
-      <c r="Z12" s="20">
+      <c r="AE12" s="15">
         <v>0.73182999999999998</v>
       </c>
-      <c r="AA12" s="21">
+      <c r="AF12" s="16">
         <v>0.66366000000000003</v>
       </c>
+      <c r="AG12" s="31">
+        <f t="shared" si="7"/>
+        <v>0.65801333333333334</v>
+      </c>
     </row>
-    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="19">
+      <c r="B13" s="15">
         <v>0.55208000000000002</v>
       </c>
-      <c r="E13" s="2">
+      <c r="C13" s="15">
         <v>0.59103000000000006</v>
       </c>
-      <c r="F13" s="25">
+      <c r="D13" s="16">
         <v>0.67013999999999996</v>
       </c>
-      <c r="G13" s="22">
+      <c r="E13" s="29">
+        <f t="shared" si="0"/>
+        <v>0.60441666666666671</v>
+      </c>
+      <c r="F13" s="17">
         <v>0.56288000000000005</v>
       </c>
-      <c r="H13" s="2">
+      <c r="G13" s="15">
         <v>0.58016999999999996</v>
       </c>
-      <c r="I13" s="25">
+      <c r="H13" s="16">
         <v>0.61889000000000005</v>
       </c>
-      <c r="J13" s="22">
+      <c r="I13" s="29">
+        <f t="shared" si="1"/>
+        <v>0.58731333333333335</v>
+      </c>
+      <c r="J13" s="17">
         <v>0.55208000000000002</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="15">
         <v>0.65664999999999996</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="16">
         <v>0.72945000000000004</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="29">
+        <f t="shared" si="2"/>
+        <v>0.64605999999999997</v>
+      </c>
+      <c r="N13" s="17">
         <v>0.56872</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="15">
         <v>0.58523000000000003</v>
       </c>
-      <c r="O13" s="25">
+      <c r="P13" s="16">
         <v>0.65708</v>
       </c>
-      <c r="P13" s="8">
+      <c r="Q13" s="29">
+        <f t="shared" si="3"/>
+        <v>0.60367666666666675</v>
+      </c>
+      <c r="R13" s="17">
         <v>0.45511000000000001</v>
       </c>
-      <c r="Q13" s="32">
+      <c r="S13" s="15">
         <v>0.44864999999999999</v>
       </c>
-      <c r="R13" s="25">
+      <c r="T13" s="16">
         <v>0.55434000000000005</v>
       </c>
-      <c r="S13" s="8">
+      <c r="U13" s="29">
+        <f t="shared" si="4"/>
+        <v>0.48603333333333332</v>
+      </c>
+      <c r="V13" s="17">
         <v>0.45896999999999999</v>
       </c>
-      <c r="T13" s="19">
+      <c r="W13" s="15">
         <v>0.45462000000000002</v>
       </c>
-      <c r="U13" s="34">
+      <c r="X13" s="16">
         <v>0.59265999999999996</v>
       </c>
-      <c r="V13" s="22">
-        <v>1</v>
-      </c>
-      <c r="W13" s="2">
-        <v>1</v>
-      </c>
-      <c r="X13" s="34">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="24">
+      <c r="Y13" s="29">
+        <f t="shared" si="5"/>
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="Z13" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="15">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AD13" s="18">
         <v>0.49767</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="AE13" s="15">
         <v>0.53166000000000002</v>
       </c>
-      <c r="AA13" s="20">
+      <c r="AF13" s="16">
         <v>0.62387999999999999</v>
       </c>
+      <c r="AG13" s="31">
+        <f t="shared" si="7"/>
+        <v>0.55107000000000006</v>
+      </c>
     </row>
-    <row r="14" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="20">
+      <c r="B14" s="15">
         <v>0.64666000000000001</v>
       </c>
-      <c r="E14" s="19">
+      <c r="C14" s="15">
         <v>0.50224000000000002</v>
       </c>
-      <c r="F14" s="6">
+      <c r="D14" s="16">
         <v>0.55852000000000002</v>
       </c>
-      <c r="G14" s="26">
+      <c r="E14" s="29">
+        <f t="shared" si="0"/>
+        <v>0.56913999999999998</v>
+      </c>
+      <c r="F14" s="17">
         <v>0.64112999999999998</v>
       </c>
-      <c r="H14" s="19">
+      <c r="G14" s="15">
         <v>0.49685000000000001</v>
       </c>
-      <c r="I14" s="6">
+      <c r="H14" s="16">
         <v>0.56993000000000005</v>
       </c>
-      <c r="J14" s="26">
+      <c r="I14" s="29">
+        <f t="shared" si="1"/>
+        <v>0.56930333333333338</v>
+      </c>
+      <c r="J14" s="17">
         <v>0.64634000000000003</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="15">
         <v>0.58213000000000004</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="16">
         <v>0.61331999999999998</v>
       </c>
-      <c r="M14" s="26">
+      <c r="M14" s="29">
+        <f t="shared" si="2"/>
+        <v>0.61392999999999998</v>
+      </c>
+      <c r="N14" s="17">
         <v>0.65381999999999996</v>
       </c>
-      <c r="N14" s="19">
+      <c r="O14" s="15">
         <v>0.49314999999999998</v>
       </c>
-      <c r="O14" s="6">
+      <c r="P14" s="16">
         <v>0.59891000000000005</v>
       </c>
-      <c r="P14" s="26">
+      <c r="Q14" s="29">
+        <f t="shared" si="3"/>
+        <v>0.58196000000000003</v>
+      </c>
+      <c r="R14" s="17">
         <v>0.62595999999999996</v>
       </c>
-      <c r="Q14" s="19">
+      <c r="S14" s="15">
         <v>0.55252999999999997</v>
       </c>
-      <c r="R14" s="6">
+      <c r="T14" s="16">
         <v>0.56801999999999997</v>
       </c>
-      <c r="S14" s="26">
+      <c r="U14" s="29">
+        <f t="shared" si="4"/>
+        <v>0.58216999999999997</v>
+      </c>
+      <c r="V14" s="17">
         <v>0.61153999999999997</v>
       </c>
-      <c r="T14" s="19">
+      <c r="W14" s="15">
         <v>0.54873000000000005</v>
       </c>
-      <c r="U14" s="6">
+      <c r="X14" s="16">
         <v>0.56081000000000003</v>
       </c>
-      <c r="V14" s="8">
+      <c r="Y14" s="29">
+        <f t="shared" si="5"/>
+        <v>0.57369333333333339</v>
+      </c>
+      <c r="Z14" s="17">
         <v>0.62595999999999996</v>
       </c>
-      <c r="W14" s="19">
+      <c r="AA14" s="15">
         <v>0.58416999999999997</v>
       </c>
-      <c r="X14" s="25">
+      <c r="AB14" s="16">
         <v>0.64268999999999998</v>
       </c>
-      <c r="Y14" s="24">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="20">
+      <c r="AC14" s="29">
+        <f t="shared" si="6"/>
+        <v>0.61760666666666664</v>
+      </c>
+      <c r="AD14" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF14" s="16">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="31">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C16" s="14" t="s">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.68103000000000002</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0.79603000000000002</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0.82974999999999999</v>
+      </c>
+      <c r="E15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.76893666666666671</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.67952999999999997</v>
+      </c>
+      <c r="G15" s="15">
+        <v>0.80652999999999997</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0.82437000000000005</v>
+      </c>
+      <c r="I15" s="29">
+        <f t="shared" si="1"/>
+        <v>0.7701433333333334</v>
+      </c>
+      <c r="J15" s="17">
+        <v>1</v>
+      </c>
+      <c r="K15" s="15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="16">
+        <v>1</v>
+      </c>
+      <c r="M15" s="29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N15" s="17">
+        <v>0.74275000000000002</v>
+      </c>
+      <c r="O15" s="15">
+        <v>0.80201999999999996</v>
+      </c>
+      <c r="P15" s="16">
+        <v>0.84258999999999995</v>
+      </c>
+      <c r="Q15" s="29">
+        <f t="shared" si="3"/>
+        <v>0.79578666666666675</v>
+      </c>
+      <c r="R15" s="17">
+        <v>0.67003999999999997</v>
+      </c>
+      <c r="S15" s="15">
+        <v>0.80071999999999999</v>
+      </c>
+      <c r="T15" s="16">
+        <v>0.80901999999999996</v>
+      </c>
+      <c r="U15" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75992666666666653</v>
+      </c>
+      <c r="V15" s="17">
+        <v>0.67059000000000002</v>
+      </c>
+      <c r="W15" s="15">
+        <v>0.71130000000000004</v>
+      </c>
+      <c r="X15" s="16">
+        <v>0.69125000000000003</v>
+      </c>
+      <c r="Y15" s="29">
+        <f t="shared" si="5"/>
+        <v>0.6910466666666667</v>
+      </c>
+      <c r="Z15" s="17">
+        <v>0.67003999999999997</v>
+      </c>
+      <c r="AA15" s="15">
+        <v>0.80071999999999999</v>
+      </c>
+      <c r="AB15" s="16">
+        <v>0.80901999999999996</v>
+      </c>
+      <c r="AC15" s="29">
+        <f t="shared" si="6"/>
+        <v>0.75992666666666653</v>
+      </c>
+      <c r="AD15" s="18">
+        <v>0.65820999999999996</v>
+      </c>
+      <c r="AE15" s="15">
+        <v>0.80174000000000001</v>
+      </c>
+      <c r="AF15" s="16">
+        <v>0.81362000000000001</v>
+      </c>
+      <c r="AG15" s="31">
+        <f t="shared" si="7"/>
+        <v>0.75785666666666673</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0.52109000000000005</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.57784999999999997</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0.56055999999999995</v>
+      </c>
+      <c r="E16" s="29">
+        <f t="shared" ref="E16" si="8">AVERAGE(B16:D16)</f>
+        <v>0.5531666666666667</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.82630000000000003</v>
+      </c>
+      <c r="G16" s="35">
+        <v>0.57740000000000002</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0.67923</v>
+      </c>
+      <c r="I16" s="29">
+        <f t="shared" ref="I16" si="9">AVERAGE(F16:H16)</f>
+        <v>0.69431000000000009</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0.89242999999999995</v>
+      </c>
+      <c r="K16" s="15">
+        <v>0.92684999999999995</v>
+      </c>
+      <c r="L16" s="16">
+        <v>0.91435999999999995</v>
+      </c>
+      <c r="M16" s="29">
+        <f t="shared" ref="M16" si="10">AVERAGE(J16:L16)</f>
+        <v>0.91121333333333332</v>
+      </c>
+      <c r="N16" s="17">
+        <v>1</v>
+      </c>
+      <c r="O16" s="15">
+        <v>1</v>
+      </c>
+      <c r="P16" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="29">
+        <f t="shared" ref="Q16" si="11">AVERAGE(N16:P16)</f>
+        <v>1</v>
+      </c>
+      <c r="R16" s="17">
+        <v>0.60175000000000001</v>
+      </c>
+      <c r="S16" s="15">
+        <v>0.45852999999999999</v>
+      </c>
+      <c r="T16" s="16">
+        <v>0.57711000000000001</v>
+      </c>
+      <c r="U16" s="29">
+        <f t="shared" ref="U16" si="12">AVERAGE(R16:T16)</f>
+        <v>0.54579666666666671</v>
+      </c>
+      <c r="V16" s="17">
+        <v>0.70499000000000001</v>
+      </c>
+      <c r="W16" s="35">
+        <v>0.45239000000000001</v>
+      </c>
+      <c r="X16" s="34">
+        <v>0.57781000000000005</v>
+      </c>
+      <c r="Y16" s="29">
+        <f t="shared" ref="Y16" si="13">AVERAGE(V16:X16)</f>
+        <v>0.57839666666666678</v>
+      </c>
+      <c r="Z16" s="17">
+        <v>0.66086999999999996</v>
+      </c>
+      <c r="AA16" s="15">
+        <v>0.80745999999999996</v>
+      </c>
+      <c r="AB16" s="16">
+        <v>0.78847999999999996</v>
+      </c>
+      <c r="AC16" s="29">
+        <f t="shared" ref="AC16" si="14">AVERAGE(Z16:AB16)</f>
+        <v>0.75226999999999988</v>
+      </c>
+      <c r="AD16" s="18">
+        <v>0.61509999999999998</v>
+      </c>
+      <c r="AE16" s="15">
+        <v>0.75800999999999996</v>
+      </c>
+      <c r="AF16" s="16">
+        <v>0.77654000000000001</v>
+      </c>
+      <c r="AG16" s="31">
+        <f t="shared" ref="AG16" si="15">AVERAGE(AD16:AF16)</f>
+        <v>0.71655000000000013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0.44771</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0.39545999999999998</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.55906999999999996</v>
+      </c>
+      <c r="E17" s="29">
+        <f t="shared" ref="E17" si="16">AVERAGE(B17:D17)</f>
+        <v>0.46741333333333329</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.80401</v>
+      </c>
+      <c r="G17" s="35">
+        <v>0.39421</v>
+      </c>
+      <c r="H17" s="34">
+        <v>0.56455999999999995</v>
+      </c>
+      <c r="I17" s="29">
+        <f t="shared" ref="I17" si="17">AVERAGE(F17:H17)</f>
+        <v>0.5875933333333333</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0.90539999999999998</v>
+      </c>
+      <c r="K17" s="15">
+        <v>0.93938999999999995</v>
+      </c>
+      <c r="L17" s="16">
+        <v>0.91539000000000004</v>
+      </c>
+      <c r="M17" s="29">
+        <f t="shared" ref="M17" si="18">AVERAGE(J17:L17)</f>
+        <v>0.92005999999999999</v>
+      </c>
+      <c r="N17" s="17">
+        <v>1</v>
+      </c>
+      <c r="O17" s="15">
+        <v>1</v>
+      </c>
+      <c r="P17" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="29">
+        <f t="shared" ref="Q17" si="19">AVERAGE(N17:P17)</f>
+        <v>1</v>
+      </c>
+      <c r="R17" s="17">
+        <v>0.56106999999999996</v>
+      </c>
+      <c r="S17" s="15">
+        <v>0.38812999999999998</v>
+      </c>
+      <c r="T17" s="16">
+        <v>0.55342999999999998</v>
+      </c>
+      <c r="U17" s="29">
+        <f t="shared" ref="U17" si="20">AVERAGE(R17:T17)</f>
+        <v>0.50087666666666664</v>
+      </c>
+      <c r="V17" s="17">
+        <v>0.74785000000000001</v>
+      </c>
+      <c r="W17" s="35">
+        <v>0.38118999999999997</v>
+      </c>
+      <c r="X17" s="34">
+        <v>0.55479999999999996</v>
+      </c>
+      <c r="Y17" s="29">
+        <f t="shared" ref="Y17" si="21">AVERAGE(V17:X17)</f>
+        <v>0.56128</v>
+      </c>
+      <c r="Z17" s="17">
+        <v>0.70620000000000005</v>
+      </c>
+      <c r="AA17" s="15">
+        <v>0.84882999999999997</v>
+      </c>
+      <c r="AB17" s="16">
+        <v>0.84428999999999998</v>
+      </c>
+      <c r="AC17" s="29">
+        <f t="shared" ref="AC17" si="22">AVERAGE(Z17:AB17)</f>
+        <v>0.79977333333333334</v>
+      </c>
+      <c r="AD17" s="18">
+        <v>0.66752999999999996</v>
+      </c>
+      <c r="AE17" s="15">
+        <v>0.81066000000000005</v>
+      </c>
+      <c r="AF17" s="16">
+        <v>0.82691999999999999</v>
+      </c>
+      <c r="AG17" s="31">
+        <f t="shared" ref="AG17" si="23">AVERAGE(AD17:AF17)</f>
+        <v>0.76837</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0.45446999999999999</v>
+      </c>
+      <c r="C18" s="15">
+        <v>0.40679999999999999</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0.43768000000000001</v>
+      </c>
+      <c r="E18" s="29">
+        <f t="shared" ref="E18" si="24">AVERAGE(B18:D18)</f>
+        <v>0.43298333333333333</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.70742000000000005</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0.40982000000000002</v>
+      </c>
+      <c r="H18" s="36">
+        <v>0.43113000000000001</v>
+      </c>
+      <c r="I18" s="29">
+        <f t="shared" ref="I18" si="25">AVERAGE(F18:H18)</f>
+        <v>0.51612333333333338</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0.73678999999999994</v>
+      </c>
+      <c r="K18" s="15">
+        <v>0.84477000000000002</v>
+      </c>
+      <c r="L18" s="16">
+        <v>0.90290000000000004</v>
+      </c>
+      <c r="M18" s="29">
+        <f t="shared" ref="M18" si="26">AVERAGE(J18:L18)</f>
+        <v>0.82815333333333341</v>
+      </c>
+      <c r="N18" s="17">
+        <v>0.70620000000000005</v>
+      </c>
+      <c r="O18" s="15">
+        <v>0.84882999999999997</v>
+      </c>
+      <c r="P18" s="16">
+        <v>0.84569000000000005</v>
+      </c>
+      <c r="Q18" s="29">
+        <f t="shared" ref="Q18" si="27">AVERAGE(N18:P18)</f>
+        <v>0.80023999999999995</v>
+      </c>
+      <c r="R18" s="17">
+        <v>0.38833000000000001</v>
+      </c>
+      <c r="S18" s="15">
+        <v>0.34647</v>
+      </c>
+      <c r="T18" s="16">
+        <v>0.41937999999999998</v>
+      </c>
+      <c r="U18" s="29">
+        <f t="shared" ref="U18" si="28">AVERAGE(R18:T18)</f>
+        <v>0.38472666666666666</v>
+      </c>
+      <c r="V18" s="17">
+        <v>0.76051000000000002</v>
+      </c>
+      <c r="W18" s="35">
+        <v>0.34747</v>
+      </c>
+      <c r="X18" s="34">
+        <v>0.41987000000000002</v>
+      </c>
+      <c r="Y18" s="29">
+        <f t="shared" ref="Y18" si="29">AVERAGE(V18:X18)</f>
+        <v>0.50928333333333331</v>
+      </c>
+      <c r="Z18" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="15">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="16">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="29">
+        <f t="shared" ref="AC18" si="30">AVERAGE(Z18:AB18)</f>
+        <v>1</v>
+      </c>
+      <c r="AD18" s="18">
+        <v>0.75041999999999998</v>
+      </c>
+      <c r="AE18" s="15">
+        <v>0.84294000000000002</v>
+      </c>
+      <c r="AF18" s="16">
+        <v>0.84658999999999995</v>
+      </c>
+      <c r="AG18" s="31">
+        <f t="shared" ref="AG18" si="31">AVERAGE(AD18:AF18)</f>
+        <v>0.81331666666666669</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0.29052</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0.26638000000000001</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.32930999999999999</v>
+      </c>
+      <c r="E19" s="29">
+        <f t="shared" ref="E19" si="32">AVERAGE(B19:D19)</f>
+        <v>0.2954033333333333</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0.72613000000000005</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0.27810000000000001</v>
+      </c>
+      <c r="H19" s="36">
+        <v>0.32861000000000001</v>
+      </c>
+      <c r="I19" s="29">
+        <f t="shared" ref="I19" si="33">AVERAGE(F19:H19)</f>
+        <v>0.44428000000000006</v>
+      </c>
+      <c r="J19" s="17">
+        <v>1</v>
+      </c>
+      <c r="K19" s="15">
+        <v>1</v>
+      </c>
+      <c r="L19" s="16">
+        <v>1</v>
+      </c>
+      <c r="M19" s="29">
+        <f t="shared" ref="M19" si="34">AVERAGE(J19:L19)</f>
+        <v>1</v>
+      </c>
+      <c r="N19" s="17">
+        <v>0.90864</v>
+      </c>
+      <c r="O19" s="15">
+        <v>0.81303999999999998</v>
+      </c>
+      <c r="P19" s="16">
+        <v>0.79601999999999995</v>
+      </c>
+      <c r="Q19" s="29">
+        <f t="shared" ref="Q19" si="35">AVERAGE(N19:P19)</f>
+        <v>0.83923333333333339</v>
+      </c>
+      <c r="R19" s="17">
+        <v>0.35650999999999999</v>
+      </c>
+      <c r="S19" s="15">
+        <v>0.3004</v>
+      </c>
+      <c r="T19" s="16">
+        <v>0.36371999999999999</v>
+      </c>
+      <c r="U19" s="29">
+        <f t="shared" ref="U19" si="36">AVERAGE(R19:T19)</f>
+        <v>0.34020999999999996</v>
+      </c>
+      <c r="V19" s="17">
+        <v>0.45846999999999999</v>
+      </c>
+      <c r="W19" s="35">
+        <v>0.30120000000000002</v>
+      </c>
+      <c r="X19" s="34">
+        <v>0.36351</v>
+      </c>
+      <c r="Y19" s="29">
+        <f t="shared" ref="Y19" si="37">AVERAGE(V19:X19)</f>
+        <v>0.37439333333333336</v>
+      </c>
+      <c r="Z19" s="17">
+        <v>0.74922999999999995</v>
+      </c>
+      <c r="AA19" s="15">
+        <v>0.85526999999999997</v>
+      </c>
+      <c r="AB19" s="16">
+        <v>0.91317999999999999</v>
+      </c>
+      <c r="AC19" s="29">
+        <f t="shared" ref="AC19" si="38">AVERAGE(Z19:AB19)</f>
+        <v>0.83922666666666668</v>
+      </c>
+      <c r="AD19" s="18">
+        <v>0.71140999999999999</v>
+      </c>
+      <c r="AE19" s="15">
+        <v>0.83457000000000003</v>
+      </c>
+      <c r="AF19" s="16">
+        <v>0.87710999999999995</v>
+      </c>
+      <c r="AG19" s="31">
+        <f t="shared" ref="AG19" si="39">AVERAGE(AD19:AF19)</f>
+        <v>0.80769666666666673</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="H16" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="G21" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="H21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="9" t="s">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="9" t="s">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="9" t="s">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="AE24" s="32"/>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="9" t="s">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="9" t="s">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D5:AA5"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="Z6:AB6"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="B5:AF5"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:H6"/>
     <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="R6:T6"/>
     <mergeCell ref="V6:X6"/>
-    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="H21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>